<commit_message>
Updated results based on the new database
</commit_message>
<xml_diff>
--- a/Scales_database/scales_database.xlsx
+++ b/Scales_database/scales_database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5885" uniqueCount="1323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5886" uniqueCount="1325">
   <si>
     <t xml:space="preserve">Sheet</t>
   </si>
@@ -3477,6 +3477,9 @@
   </si>
   <si>
     <t xml:space="preserve">10.1121/1.2828063</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.2307/927751 </t>
   </si>
   <si>
     <t xml:space="preserve">Aning, Ben, tuning the kora: a case study of the norms of a gambian musician</t>
@@ -3871,6 +3874,9 @@
     <t xml:space="preserve">Despite noting in the text that the octave, the final interval leading to the octave is not reported. In this case I assume that the octave is perfect, and insert the missing interval.</t>
   </si>
   <si>
+    <t xml:space="preserve">Gilbert Rouget and J. Schwarz. Sur les xylophones quiheptaphoniques des malink. Rev. Musicol., 55(1):47–77, 1969. doi: 10.2307/927751</t>
+  </si>
+  <si>
     <t xml:space="preserve">A. Tracey. The matepe mbira music of rhodesia. Afr. Music, 4(4):37–61, 1970. doi: 10.21504/amj.v4i4.1681</t>
   </si>
   <si>
@@ -3943,7 +3949,9 @@
     <t xml:space="preserve">L. E. McNeil and S. Mitran. Vibrational frequencies and tuning of the african mbira. J. Acoust. Soc. Am., 123(2):1169–1178, 2008. doi: 10.1121/1.2828063</t>
   </si>
   <si>
-    <t xml:space="preserve">Multiple octaves were recorded as separate scales for each xylophone for two reasons. First, the notes are numbered. Second, there is substantial variation between octaves to consider them as distinct versions of the same scale.</t>
+    <t xml:space="preserve">Multiple octaves were recorded as separate scales for each xylophone for two reasons.
+First, the notes are numbered, so the notes can be arranged in the correct order.
+Second, there is substantial variation between octaves to consider them as distinct versions of the same scale.</t>
   </si>
   <si>
     <t xml:space="preserve">M. Kuss. Music in Latin America and the Caribbean: An Encyclopedic History: Volume 1: Performing Beliefs: Indigenous Peoples of South America, Central America, and Mexico. University of Texas Press, 2010</t>
@@ -4199,7 +4207,7 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -4304,8 +4312,8 @@
   </sheetPr>
   <dimension ref="A1:I467"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A313" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I326" activeCellId="0" sqref="I326"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A351" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H355" activeCellId="0" sqref="H355"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14526,7 +14534,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="353" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="5" t="s">
         <v>775</v>
       </c>
@@ -14555,7 +14563,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="354" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="5" t="s">
         <v>777</v>
       </c>
@@ -14578,7 +14586,7 @@
         <v>28</v>
       </c>
       <c r="H354" s="0" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I354" s="0" t="s">
         <v>29</v>
@@ -14607,7 +14615,7 @@
         <v>28</v>
       </c>
       <c r="H355" s="0" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I355" s="0" t="s">
         <v>29</v>
@@ -14636,13 +14644,13 @@
         <v>28</v>
       </c>
       <c r="H356" s="0" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I356" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="357" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="5" t="s">
         <v>782</v>
       </c>
@@ -14665,13 +14673,13 @@
         <v>28</v>
       </c>
       <c r="H357" s="0" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I357" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="358" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="5" t="s">
         <v>783</v>
       </c>
@@ -14694,13 +14702,13 @@
         <v>28</v>
       </c>
       <c r="H358" s="0" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I358" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="359" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="5" t="s">
         <v>784</v>
       </c>
@@ -14723,13 +14731,13 @@
         <v>28</v>
       </c>
       <c r="H359" s="0" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I359" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="360" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="5" t="s">
         <v>785</v>
       </c>
@@ -14752,13 +14760,13 @@
         <v>28</v>
       </c>
       <c r="H360" s="0" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I360" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="361" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="5" t="s">
         <v>786</v>
       </c>
@@ -14781,13 +14789,13 @@
         <v>28</v>
       </c>
       <c r="H361" s="0" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I361" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="362" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="5" t="s">
         <v>787</v>
       </c>
@@ -14810,13 +14818,13 @@
         <v>28</v>
       </c>
       <c r="H362" s="0" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I362" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="363" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="5" t="s">
         <v>788</v>
       </c>
@@ -14839,13 +14847,13 @@
         <v>28</v>
       </c>
       <c r="H363" s="0" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I363" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="364" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="5" t="s">
         <v>789</v>
       </c>
@@ -14868,13 +14876,13 @@
         <v>28</v>
       </c>
       <c r="H364" s="0" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I364" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="365" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="5" t="s">
         <v>790</v>
       </c>
@@ -14897,13 +14905,13 @@
         <v>28</v>
       </c>
       <c r="H365" s="0" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I365" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="366" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="5" t="s">
         <v>791</v>
       </c>
@@ -14926,13 +14934,13 @@
         <v>28</v>
       </c>
       <c r="H366" s="0" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I366" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="367" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="5" t="s">
         <v>792</v>
       </c>
@@ -14955,7 +14963,7 @@
         <v>28</v>
       </c>
       <c r="H367" s="0" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I367" s="0" t="s">
         <v>29</v>
@@ -19534,8 +19542,8 @@
   </sheetPr>
   <dimension ref="A1:GZ31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="GJ1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="GZ5" activeCellId="0" sqref="GZ5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="FY1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="GK9" activeCellId="0" sqref="GK9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22448,10 +22456,10 @@
         <v>1117</v>
       </c>
       <c r="ED5" s="0" t="s">
-        <v>1118</v>
+        <v>1134</v>
       </c>
       <c r="EE5" s="0" t="s">
-        <v>1118</v>
+        <v>1134</v>
       </c>
       <c r="EF5" s="0" t="s">
         <v>1134</v>
@@ -22906,789 +22914,789 @@
         <v>1149</v>
       </c>
       <c r="BZ6" s="0" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="CA6" s="0" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="CB6" s="0" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="CC6" s="0" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="CD6" s="0" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="CE6" s="6" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="CF6" s="6" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="CG6" s="6" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="CH6" s="6" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="CI6" s="6" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="CJ6" s="6" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="CK6" s="6" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="CL6" s="6" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="CM6" s="6" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="CN6" s="6" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="CO6" s="6" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="CP6" s="6" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="CQ6" s="6" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="CR6" s="6" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="CS6" s="0" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="CT6" s="0" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="CU6" s="0" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="CV6" s="0" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="CW6" s="0" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="CX6" s="0" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="CY6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="CZ6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DA6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DB6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DC6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DD6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DE6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DF6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DG6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DH6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DI6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DJ6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DK6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DL6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DM6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DN6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DO6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DP6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DQ6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DR6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DS6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DT6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DU6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DV6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DW6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DX6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DY6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="DZ6" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="EA6" s="6" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="EB6" s="6" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="EC6" s="6" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="ED6" s="6" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="EE6" s="6" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="EF6" s="6" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="EG6" s="6" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="EH6" s="6" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="EI6" s="6" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="EJ6" s="6" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="EK6" s="6" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="EL6" s="6" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="EM6" s="6" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="EN6" s="6" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="EO6" s="6" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="EP6" s="0" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="EQ6" s="0" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="ER6" s="0" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="ES6" s="0" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="ET6" s="0" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="EU6" s="0" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="EV6" s="0" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="EW6" s="0" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="EX6" s="0" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="EY6" s="0" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="EZ6" s="0" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="FA6" s="0" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="FB6" s="0" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="FC6" s="0" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="FD6" s="0" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="FE6" s="0" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="FF6" s="0" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="FG6" s="0" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="FH6" s="0" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="FI6" s="0" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="FJ6" s="0" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="FK6" s="0" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="FL6" s="0" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="FM6" s="0" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="FN6" s="0" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="FO6" s="0" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="FP6" s="0" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="FQ6" s="0" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="FR6" s="0" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="FS6" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="FT6" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="FU6" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="FV6" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="FW6" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="FX6" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="FY6" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="FZ6" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="GA6" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="GB6" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="GC6" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="GD6" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="GE6" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="GF6" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="GG6" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="GH6" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="GI6" s="3" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="GJ6" s="3" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="GK6" s="3" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="GL6" s="3" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="GM6" s="3" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="GN6" s="3" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="GO6" s="3" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="GP6" s="0" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="GQ6" s="0" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="GR6" s="0" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="GS6" s="0" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="GT6" s="0" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="GU6" s="0" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="GV6" s="0" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="GW6" s="0" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="GX6" s="0" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="GY6" s="0" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="GZ6" s="0" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G7" s="6" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H7" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="J7" s="6" t="n">
         <v>27</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="K7" s="6" t="n">
         <v>27</v>
       </c>
-      <c r="J7" s="6" t="n">
+      <c r="L7" s="6" t="n">
         <v>26</v>
       </c>
-      <c r="K7" s="6" t="n">
+      <c r="M7" s="6" t="n">
         <v>26</v>
       </c>
-      <c r="L7" s="6" t="n">
+      <c r="N7" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="O7" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="P7" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q7" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="R7" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="S7" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="T7" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="U7" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="V7" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="W7" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="X7" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y7" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="Z7" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="AA7" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="AB7" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="AC7" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="AD7" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="AE7" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="AF7" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="AG7" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="AH7" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="AI7" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="AJ7" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="AK7" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="AL7" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="AM7" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="AN7" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="AO7" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="AP7" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="AQ7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="AR7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="AS7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="AT7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="AU7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="AV7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="AW7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="AX7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="AY7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="AZ7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="BA7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="BB7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="BC7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="BD7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="BE7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="BF7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="BG7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="BH7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="BI7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="BJ7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="BK7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="BL7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="BM7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="BN7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="BO7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="BP7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="BQ7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="BR7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="BS7" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="BT7" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="BU7" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="BV7" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="BW7" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="BX7" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="M7" s="6" t="n">
-        <v>25</v>
-      </c>
-      <c r="N7" s="6" t="n">
-        <v>29</v>
-      </c>
-      <c r="O7" s="6" t="n">
-        <v>29</v>
-      </c>
-      <c r="P7" s="6" t="n">
-        <v>29</v>
-      </c>
-      <c r="Q7" s="6" t="n">
-        <v>29</v>
-      </c>
-      <c r="R7" s="6" t="n">
-        <v>29</v>
-      </c>
-      <c r="S7" s="6" t="n">
-        <v>29</v>
-      </c>
-      <c r="T7" s="6" t="n">
-        <v>29</v>
-      </c>
-      <c r="U7" s="6" t="n">
-        <v>29</v>
-      </c>
-      <c r="V7" s="6" t="n">
-        <v>29</v>
-      </c>
-      <c r="W7" s="6" t="n">
-        <v>29</v>
-      </c>
-      <c r="X7" s="6" t="n">
-        <v>29</v>
-      </c>
-      <c r="Y7" s="6" t="n">
-        <v>29</v>
-      </c>
-      <c r="Z7" s="6" t="n">
-        <v>13</v>
-      </c>
-      <c r="AA7" s="6" t="n">
-        <v>13</v>
-      </c>
-      <c r="AB7" s="6" t="n">
-        <v>13</v>
-      </c>
-      <c r="AC7" s="6" t="n">
-        <v>13</v>
-      </c>
-      <c r="AD7" s="6" t="n">
-        <v>13</v>
-      </c>
-      <c r="AE7" s="6" t="n">
-        <v>13</v>
-      </c>
-      <c r="AF7" s="6" t="n">
-        <v>13</v>
-      </c>
-      <c r="AG7" s="6" t="n">
-        <v>13</v>
-      </c>
-      <c r="AH7" s="6" t="n">
-        <v>13</v>
-      </c>
-      <c r="AI7" s="6" t="n">
-        <v>16</v>
-      </c>
-      <c r="AJ7" s="6" t="n">
-        <v>16</v>
-      </c>
-      <c r="AK7" s="6" t="n">
-        <v>16</v>
-      </c>
-      <c r="AL7" s="6" t="n">
-        <v>16</v>
-      </c>
-      <c r="AM7" s="6" t="n">
-        <v>16</v>
-      </c>
-      <c r="AN7" s="6" t="n">
-        <v>16</v>
-      </c>
-      <c r="AO7" s="6" t="n">
-        <v>16</v>
-      </c>
-      <c r="AP7" s="6" t="n">
-        <v>16</v>
-      </c>
-      <c r="AQ7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="AR7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="AS7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="AT7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="AU7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="AV7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="AW7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="AX7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="AY7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="AZ7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="BA7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="BB7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="BC7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="BD7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="BE7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="BF7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="BG7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="BH7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="BI7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="BJ7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="BK7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="BL7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="BM7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="BN7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="BO7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="BP7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="BQ7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="BR7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="BS7" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="BT7" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="BU7" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="BV7" s="0" t="n">
+      <c r="BY7" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="BZ7" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="BW7" s="0" t="n">
+      <c r="CA7" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="BX7" s="0" t="n">
+      <c r="CB7" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="CC7" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="CD7" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="CE7" s="6" t="n">
         <v>24</v>
       </c>
-      <c r="BY7" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="BZ7" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="CA7" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="CB7" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="CC7" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="CD7" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="CE7" s="6" t="n">
+      <c r="CF7" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="CG7" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="CH7" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="CI7" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="CJ7" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="CF7" s="6" t="n">
+      <c r="CK7" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="CG7" s="6" t="n">
+      <c r="CL7" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="CH7" s="6" t="n">
+      <c r="CM7" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="CI7" s="6" t="n">
-        <v>23</v>
-      </c>
-      <c r="CJ7" s="6" t="n">
-        <v>22</v>
-      </c>
-      <c r="CK7" s="6" t="n">
-        <v>22</v>
-      </c>
-      <c r="CL7" s="6" t="n">
-        <v>22</v>
-      </c>
-      <c r="CM7" s="6" t="n">
-        <v>22</v>
-      </c>
       <c r="CN7" s="6" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="CO7" s="6" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="CP7" s="6" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="CQ7" s="6" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="CR7" s="6" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="CS7" s="0" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="CT7" s="0" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="CU7" s="0" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="CV7" s="0" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="CW7" s="0" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="CX7" s="0" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="CY7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="CZ7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DA7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DB7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DC7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DD7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DE7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DF7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DG7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DH7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DI7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DJ7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DK7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DL7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DM7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DN7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DO7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DP7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DQ7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DR7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DS7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DT7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DU7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DV7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DW7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DX7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DY7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="DZ7" s="6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="EA7" s="6" t="n">
         <v>4</v>
@@ -23697,10 +23705,10 @@
         <v>4</v>
       </c>
       <c r="EC7" s="6" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="ED7" s="6" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="EE7" s="6" t="n">
         <v>5</v>
@@ -23715,112 +23723,112 @@
         <v>5</v>
       </c>
       <c r="EI7" s="6" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="EJ7" s="6" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="EK7" s="6" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="EL7" s="6" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="EM7" s="6" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="EN7" s="6" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="EO7" s="6" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="EP7" s="0" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="EQ7" s="0" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="ER7" s="0" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="ES7" s="0" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="ET7" s="0" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="EU7" s="0" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="EV7" s="0" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="EW7" s="0" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="EX7" s="0" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="EY7" s="0" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="EZ7" s="0" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="FA7" s="0" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="FB7" s="0" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="FC7" s="0" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="FD7" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="FE7" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="FF7" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="FG7" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="FH7" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="FI7" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="FJ7" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="FK7" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="FL7" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="FM7" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="FN7" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="FO7" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="FP7" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="FQ7" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="FR7" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="FS7" s="3" t="n">
         <v>6</v>
@@ -23871,25 +23879,25 @@
         <v>6</v>
       </c>
       <c r="GI7" s="3" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="GJ7" s="3" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="GK7" s="3" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="GL7" s="3" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="GM7" s="3" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="GN7" s="3" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="GO7" s="3" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="GP7" s="0" t="n">
         <v>7</v>
@@ -29770,7 +29778,7 @@
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="M53" activeCellId="0" sqref="M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29826,7 +29834,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="B2" s="8" t="n">
         <v>307</v>
@@ -29859,7 +29867,7 @@
         <v>858</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="M2" s="0" t="n">
         <v>11</v>
@@ -29870,7 +29878,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="B3" s="8" t="n">
         <v>306</v>
@@ -29903,7 +29911,7 @@
         <v>858</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="M3" s="0" t="n">
         <v>11</v>
@@ -29914,7 +29922,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="B4" s="8" t="n">
         <v>297</v>
@@ -29947,7 +29955,7 @@
         <v>858</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="M4" s="0" t="n">
         <v>11</v>
@@ -29958,7 +29966,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="B5" s="8" t="n">
         <v>295</v>
@@ -29991,7 +29999,7 @@
         <v>858</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="M5" s="0" t="n">
         <v>11</v>
@@ -30002,7 +30010,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="B6" s="8" t="n">
         <v>298</v>
@@ -30035,7 +30043,7 @@
         <v>858</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="M6" s="0" t="n">
         <v>11</v>
@@ -30046,7 +30054,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="B7" s="8" t="n">
         <v>292</v>
@@ -30079,7 +30087,7 @@
         <v>858</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="M7" s="0" t="n">
         <v>11</v>
@@ -30090,7 +30098,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="B8" s="8" t="n">
         <v>295</v>
@@ -30123,7 +30131,7 @@
         <v>858</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="M8" s="0" t="n">
         <v>11</v>
@@ -30134,7 +30142,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="B9" s="8" t="n">
         <v>294</v>
@@ -30167,7 +30175,7 @@
         <v>858</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="M9" s="0" t="n">
         <v>11</v>
@@ -30178,7 +30186,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="B10" s="8" t="n">
         <v>293</v>
@@ -30211,7 +30219,7 @@
         <v>858</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="M10" s="0" t="n">
         <v>11</v>
@@ -30222,7 +30230,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="B11" s="8" t="n">
         <v>286</v>
@@ -30255,7 +30263,7 @@
         <v>858</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="M11" s="0" t="n">
         <v>11</v>
@@ -30266,7 +30274,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="B12" s="8" t="n">
         <v>287</v>
@@ -30299,7 +30307,7 @@
         <v>858</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="M12" s="0" t="n">
         <v>11</v>
@@ -30310,7 +30318,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="B13" s="3" t="n">
         <v>286</v>
@@ -30343,7 +30351,7 @@
         <v>858</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="M13" s="0" t="n">
         <v>11</v>
@@ -30354,7 +30362,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="B14" s="3" t="n">
         <v>276</v>
@@ -30387,7 +30395,7 @@
         <v>858</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="M14" s="0" t="n">
         <v>11</v>
@@ -30398,7 +30406,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="B15" s="3" t="n">
         <v>276</v>
@@ -30431,7 +30439,7 @@
         <v>858</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="M15" s="0" t="n">
         <v>11</v>
@@ -30442,7 +30450,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="B16" s="3" t="n">
         <v>275</v>
@@ -30475,7 +30483,7 @@
         <v>858</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="M16" s="0" t="n">
         <v>11</v>
@@ -30486,7 +30494,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="B17" s="3" t="n">
         <v>276</v>
@@ -30519,7 +30527,7 @@
         <v>858</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="M17" s="0" t="n">
         <v>11</v>
@@ -30530,7 +30538,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="B18" s="3" t="n">
         <v>272</v>
@@ -30563,7 +30571,7 @@
         <v>858</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="M18" s="0" t="n">
         <v>11</v>
@@ -30574,7 +30582,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="B19" s="3" t="n">
         <v>273</v>
@@ -30607,7 +30615,7 @@
         <v>858</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="M19" s="0" t="n">
         <v>11</v>
@@ -30618,7 +30626,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="B20" s="3" t="n">
         <v>268</v>
@@ -30651,7 +30659,7 @@
         <v>858</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="M20" s="0" t="n">
         <v>11</v>
@@ -30662,7 +30670,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="B21" s="3" t="n">
         <v>261</v>
@@ -30695,7 +30703,7 @@
         <v>858</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="M21" s="0" t="n">
         <v>11</v>
@@ -30706,7 +30714,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="B22" s="3" t="n">
         <v>216</v>
@@ -30739,7 +30747,7 @@
         <v>858</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="M22" s="0" t="n">
         <v>11</v>
@@ -30750,7 +30758,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="B23" s="3" t="n">
         <v>214</v>
@@ -30783,7 +30791,7 @@
         <v>858</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="M23" s="0" t="n">
         <v>11</v>
@@ -30794,7 +30802,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="B24" s="3" t="n">
         <v>198</v>
@@ -30827,7 +30835,7 @@
         <v>858</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="M24" s="0" t="n">
         <v>11</v>
@@ -30838,7 +30846,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="B25" s="8" t="n">
         <v>306</v>
@@ -30871,7 +30879,7 @@
         <v>858</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M25" s="0" t="n">
         <v>11</v>
@@ -30882,7 +30890,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="B26" s="8" t="n">
         <v>296</v>
@@ -30915,7 +30923,7 @@
         <v>858</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M26" s="0" t="n">
         <v>11</v>
@@ -30926,7 +30934,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="B27" s="8" t="n">
         <v>293</v>
@@ -30959,7 +30967,7 @@
         <v>858</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M27" s="0" t="n">
         <v>11</v>
@@ -30970,7 +30978,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="B28" s="8" t="n">
         <v>289</v>
@@ -31003,7 +31011,7 @@
         <v>858</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M28" s="0" t="n">
         <v>11</v>
@@ -31014,7 +31022,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="B29" s="8" t="n">
         <v>288</v>
@@ -31047,7 +31055,7 @@
         <v>858</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M29" s="0" t="n">
         <v>11</v>
@@ -31058,7 +31066,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="B30" s="8" t="n">
         <v>281</v>
@@ -31091,7 +31099,7 @@
         <v>858</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M30" s="0" t="n">
         <v>11</v>
@@ -31102,7 +31110,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="B31" s="8" t="n">
         <v>279</v>
@@ -31135,7 +31143,7 @@
         <v>858</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M31" s="0" t="n">
         <v>11</v>
@@ -31146,7 +31154,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="B32" s="8" t="n">
         <v>278</v>
@@ -31179,7 +31187,7 @@
         <v>858</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M32" s="0" t="n">
         <v>11</v>
@@ -31190,7 +31198,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="B33" s="8" t="n">
         <v>274</v>
@@ -31223,7 +31231,7 @@
         <v>858</v>
       </c>
       <c r="L33" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M33" s="0" t="n">
         <v>11</v>
@@ -31234,7 +31242,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="B34" s="8" t="n">
         <v>274</v>
@@ -31267,7 +31275,7 @@
         <v>858</v>
       </c>
       <c r="L34" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M34" s="0" t="n">
         <v>11</v>
@@ -31278,7 +31286,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="B35" s="8" t="n">
         <v>273</v>
@@ -31311,7 +31319,7 @@
         <v>858</v>
       </c>
       <c r="L35" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M35" s="0" t="n">
         <v>11</v>
@@ -31322,7 +31330,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="B36" s="8" t="n">
         <v>273</v>
@@ -31355,7 +31363,7 @@
         <v>858</v>
       </c>
       <c r="L36" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M36" s="0" t="n">
         <v>11</v>
@@ -31366,7 +31374,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="B37" s="8" t="n">
         <v>273</v>
@@ -31399,7 +31407,7 @@
         <v>858</v>
       </c>
       <c r="L37" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M37" s="0" t="n">
         <v>11</v>
@@ -31410,7 +31418,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="B38" s="8" t="n">
         <v>269</v>
@@ -31443,7 +31451,7 @@
         <v>858</v>
       </c>
       <c r="L38" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M38" s="0" t="n">
         <v>11</v>
@@ -31454,7 +31462,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="B39" s="8" t="n">
         <v>272</v>
@@ -31487,7 +31495,7 @@
         <v>858</v>
       </c>
       <c r="L39" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M39" s="0" t="n">
         <v>11</v>
@@ -31498,7 +31506,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="B40" s="8" t="n">
         <v>270</v>
@@ -31531,7 +31539,7 @@
         <v>858</v>
       </c>
       <c r="L40" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M40" s="0" t="n">
         <v>11</v>
@@ -31542,7 +31550,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="B41" s="8" t="n">
         <v>268</v>
@@ -31575,7 +31583,7 @@
         <v>858</v>
       </c>
       <c r="L41" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M41" s="0" t="n">
         <v>11</v>
@@ -31586,7 +31594,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B42" s="8" t="n">
         <v>270</v>
@@ -31619,7 +31627,7 @@
         <v>858</v>
       </c>
       <c r="L42" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M42" s="0" t="n">
         <v>11</v>
@@ -31630,7 +31638,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="B43" s="8" t="n">
         <v>267</v>
@@ -31663,7 +31671,7 @@
         <v>858</v>
       </c>
       <c r="L43" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M43" s="0" t="n">
         <v>11</v>
@@ -31674,7 +31682,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="B44" s="8" t="n">
         <v>267</v>
@@ -31707,7 +31715,7 @@
         <v>858</v>
       </c>
       <c r="L44" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M44" s="0" t="n">
         <v>11</v>
@@ -31718,7 +31726,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="B45" s="8" t="n">
         <v>265</v>
@@ -31751,7 +31759,7 @@
         <v>858</v>
       </c>
       <c r="L45" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M45" s="0" t="n">
         <v>11</v>
@@ -31762,7 +31770,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="B46" s="8" t="n">
         <v>264</v>
@@ -31795,7 +31803,7 @@
         <v>858</v>
       </c>
       <c r="L46" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M46" s="0" t="n">
         <v>11</v>
@@ -31806,7 +31814,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="B47" s="8" t="n">
         <v>263</v>
@@ -31839,7 +31847,7 @@
         <v>858</v>
       </c>
       <c r="L47" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M47" s="0" t="n">
         <v>11</v>
@@ -31850,7 +31858,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="B48" s="8" t="n">
         <v>260</v>
@@ -31883,7 +31891,7 @@
         <v>858</v>
       </c>
       <c r="L48" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M48" s="0" t="n">
         <v>11</v>
@@ -31894,7 +31902,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="B49" s="8" t="n">
         <v>259</v>
@@ -31927,7 +31935,7 @@
         <v>858</v>
       </c>
       <c r="L49" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M49" s="0" t="n">
         <v>11</v>
@@ -31938,7 +31946,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="B50" s="8" t="n">
         <v>261</v>
@@ -31971,7 +31979,7 @@
         <v>858</v>
       </c>
       <c r="L50" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M50" s="0" t="n">
         <v>11</v>
@@ -31982,7 +31990,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="B51" s="8" t="n">
         <v>259</v>
@@ -32015,7 +32023,7 @@
         <v>858</v>
       </c>
       <c r="L51" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M51" s="0" t="n">
         <v>11</v>
@@ -32026,7 +32034,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="B52" s="8" t="n">
         <v>246</v>
@@ -32059,7 +32067,7 @@
         <v>858</v>
       </c>
       <c r="L52" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="M52" s="0" t="n">
         <v>11</v>
@@ -32086,8 +32094,8 @@
   </sheetPr>
   <dimension ref="A1:BB21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AZ7" activeCellId="0" sqref="AZ7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K35" activeCellId="0" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -32097,166 +32105,166 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>132</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="Z1" s="0" t="s">
         <v>983</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="AG1" s="0" t="s">
+        <v>1247</v>
+      </c>
+      <c r="AH1" s="0" t="s">
         <v>1246</v>
       </c>
-      <c r="AH1" s="0" t="s">
-        <v>1245</v>
-      </c>
       <c r="AI1" s="0" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="AL1" s="0" t="s">
         <v>856</v>
       </c>
       <c r="AM1" s="0" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="AO1" s="0" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="AP1" s="0" t="s">
         <v>862</v>
       </c>
       <c r="AQ1" s="0" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="AR1" s="0" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="AS1" s="0" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="AT1" s="0" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="AU1" s="0" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="AV1" s="0" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="AW1" s="0" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="AX1" s="0" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="AY1" s="0" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="AZ1" s="0" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="BA1" s="0" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="BB1" s="0" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32503,28 +32511,28 @@
         <v>408</v>
       </c>
       <c r="AA3" s="5" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="AB3" s="5" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="AC3" s="5" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="AD3" s="5" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="AE3" s="0" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="AF3" s="0" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="AG3" s="0" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="AH3" s="0" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="AI3" s="0" t="s">
         <v>928</v>
@@ -32578,13 +32586,13 @@
         <v>763</v>
       </c>
       <c r="AZ3" s="0" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="BA3" s="0" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="BB3" s="0" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32828,7 +32836,7 @@
         <v>29</v>
       </c>
       <c r="Z5" s="0" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="AA5" s="0" t="s">
         <v>937</v>
@@ -32852,7 +32860,7 @@
         <v>937</v>
       </c>
       <c r="AH5" s="0" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="AI5" s="0" t="s">
         <v>928</v>
@@ -32906,177 +32914,177 @@
         <v>763</v>
       </c>
       <c r="AZ5" s="0" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="BA5" s="0" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="BB5" s="0" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="S6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="T6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="U6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="V6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="W6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="X6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="Y6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="Z6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AA6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AB6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AC6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AD6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AE6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AF6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AG6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AH6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AI6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AJ6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AK6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AL6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AM6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AN6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AO6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AP6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AQ6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AR6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AS6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AT6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AU6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AV6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AW6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AX6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AY6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AZ6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="BA6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="BB6" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34491,7 +34499,7 @@
         <v>191</v>
       </c>
       <c r="AF16" s="0" t="n">
-        <v>321</v>
+        <v>180</v>
       </c>
       <c r="AG16" s="0" t="n">
         <v>205</v>
@@ -34514,7 +34522,7 @@
         <v>100</v>
       </c>
       <c r="AF17" s="0" t="n">
-        <v>355</v>
+        <v>167</v>
       </c>
       <c r="AG17" s="0" t="n">
         <v>173</v>
@@ -34534,7 +34542,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AF18" s="0" t="n">
-        <v>391</v>
+        <v>181</v>
       </c>
       <c r="AG18" s="0" t="n">
         <v>150</v>
@@ -34545,7 +34553,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AF19" s="0" t="n">
-        <v>434</v>
+        <v>189</v>
       </c>
       <c r="AG19" s="0" t="n">
         <v>195</v>
@@ -34553,7 +34561,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AF20" s="0" t="n">
-        <v>484</v>
+        <v>160</v>
       </c>
       <c r="AG20" s="0" t="n">
         <v>221</v>
@@ -34561,7 +34569,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AF21" s="0" t="n">
-        <v>531</v>
+        <v>159</v>
       </c>
       <c r="AG21" s="0" t="n">
         <v>160</v>
@@ -34583,10 +34591,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -34599,13 +34607,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>20</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34613,7 +34621,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34621,10 +34629,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34632,10 +34640,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34643,7 +34651,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34651,10 +34659,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34662,7 +34670,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34670,7 +34678,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34678,7 +34686,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34686,23 +34694,23 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>1167</v>
+      <c r="B11" s="0" t="s">
+        <v>1282</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>1281</v>
+      <c r="B12" s="3" t="s">
+        <v>1168</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34710,7 +34718,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34718,7 +34726,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34726,7 +34734,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34734,7 +34742,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34742,7 +34750,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34750,7 +34758,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34758,9 +34766,6 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>1288</v>
-      </c>
-      <c r="C19" s="0" t="s">
         <v>1289</v>
       </c>
     </row>
@@ -34771,13 +34776,16 @@
       <c r="B20" s="0" t="s">
         <v>1290</v>
       </c>
+      <c r="C20" s="0" t="s">
+        <v>1291</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="n">
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34785,10 +34793,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>1292</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>1278</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34796,7 +34801,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>1293</v>
+        <v>1294</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>1279</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34804,10 +34812,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>1294</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>1278</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34815,7 +34820,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>1295</v>
+        <v>1296</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>1279</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34823,7 +34831,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34831,7 +34839,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34839,7 +34847,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34847,9 +34855,6 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>1299</v>
-      </c>
-      <c r="C29" s="0" t="s">
         <v>1300</v>
       </c>
     </row>
@@ -34859,6 +34864,9 @@
       </c>
       <c r="B30" s="0" t="s">
         <v>1301</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>1302</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34866,7 +34874,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34874,18 +34882,18 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>1303</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="36.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11" t="n">
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>1304</v>
+        <v>1166</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>1305</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34893,15 +34901,15 @@
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>1305</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="11" t="n">
         <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34909,7 +34917,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34917,7 +34925,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34925,9 +34933,6 @@
         <v>37</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>1309</v>
-      </c>
-      <c r="C38" s="0" t="s">
         <v>1310</v>
       </c>
     </row>
@@ -34939,18 +34944,29 @@
         <v>1311</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>1310</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="n">
         <v>39</v>
       </c>
       <c r="B40" s="0" t="s">
+        <v>1313</v>
+      </c>
+      <c r="C40" s="0" t="s">
         <v>1312</v>
       </c>
-      <c r="C40" s="5" t="s">
-        <v>1313</v>
+    </row>
+    <row r="41" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="11" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>1314</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>1315</v>
       </c>
     </row>
   </sheetData>
@@ -34971,8 +34987,8 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -34984,7 +35000,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
-        <v>1314</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34992,7 +35008,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1315</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35000,7 +35016,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>1316</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35008,7 +35024,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>1317</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35016,7 +35032,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>1318</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35024,7 +35040,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>1319</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35032,7 +35048,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>1320</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35040,7 +35056,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>1321</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35048,7 +35064,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>1322</v>
+        <v>1324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Statistics and octave analysis
</commit_message>
<xml_diff>
--- a/Scales_database/scales_database.xlsx
+++ b/Scales_database/scales_database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5886" uniqueCount="1325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6001" uniqueCount="1383">
   <si>
     <t xml:space="preserve">Sheet</t>
   </si>
@@ -3842,10 +3842,25 @@
     <t xml:space="preserve">Number</t>
   </si>
   <si>
-    <t xml:space="preserve">Notes</t>
+    <t xml:space="preserve">Measurement device(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes on the inclusion of scales in the database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supports octave equivalence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes on octave equivalence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other Notes</t>
   </si>
   <si>
     <t xml:space="preserve">M. J. Hewitt. Musical Scales of the World. Note Tree, 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?</t>
   </si>
   <si>
     <t xml:space="preserve">H. Rechberger. Scales and Modes Around the World: The Complete Guide to the Scales and Modes of the World. Fennica Gehrman Ltd., 2018</t>
@@ -3868,85 +3883,217 @@
     <t xml:space="preserve">K. P. Wachsmann. An equal-stepped tuning in a ganda harp. Nature, 165(4184):40–41, 1950. doi: 10.1038/165040a0</t>
   </si>
   <si>
+    <t xml:space="preserve">Stroboconn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is noted that multiple strings are supposed to be an octave apart, and that “good octaves are the hallmark of the efficient tuner”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equidistance in tuning comes from matching the interval sizes between strings – it seems to be a choice</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gerhard Kubik. Harp music of the azande and related peoples in the central african republic: (part i horizontal harp playing). Afr. Music, 3(3):37–76, 1964</t>
   </si>
   <si>
     <t xml:space="preserve">Despite noting in the text that the octave, the final interval leading to the octave is not reported. In this case I assume that the octave is perfect, and insert the missing interval.</t>
   </si>
   <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Contrary movement from unison into octave and the reverse is a frequent practice in Azande harp music”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Each player seems to tune his instrument to fit best the range of his voice and that of the choir”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monochord</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“If men and women sing together the result is generally in parallel octaves”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not mentioned clearly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Seldom does the interval go beyond one full tone and rarely does the compass of a song contain more than one octave.”</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gilbert Rouget and J. Schwarz. Sur les xylophones quiheptaphoniques des malink. Rev. Musicol., 55(1):47–77, 1969. doi: 10.2307/927751</t>
   </si>
   <si>
+    <t xml:space="preserve">French.. ask Francois</t>
+  </si>
+  <si>
     <t xml:space="preserve">A. Tracey. The matepe mbira music of rhodesia. Afr. Music, 4(4):37–61, 1970. doi: 10.21504/amj.v4i4.1681</t>
   </si>
   <si>
+    <t xml:space="preserve">Makes reference to “octave transpositions”; “all seven index reeds are often played in octave unison”</t>
+  </si>
+  <si>
     <t xml:space="preserve">A. Tracey. The nyanga panpipe dance. Afr. Music, 5(1):73–89, 1971. doi: 10.21504/amj.v5i1.1152</t>
   </si>
   <si>
+    <t xml:space="preserve">“In common with other reedpipe dances that have been described, the maker does not tune according to an abstracted scale. He does not tune each note in turn up or down the scale, and he does not specifically tune together the same notes on different panpipes, or check octaves or fifths. The only method seems to be to play the actual music that belongs to it, on a set that is to be tuned, and see if it fits with what is expected. Then two different panpipes of a similar pitch range are tested together, and so on through the set. For testing any particular panpipe, the one most often chosen to play against it is the one that stands next to it during the dance.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 cents resolution given, but no measurement device specified</t>
+  </si>
+  <si>
     <t xml:space="preserve">W. Surjodiningrat, A. Susanto, and P. J. Sudarjana. Tone Measurements of Outstanding Javanese Gamelans in Jogjakarta and Surakarta. Gadjah Mada University Press, 1972</t>
   </si>
   <si>
     <t xml:space="preserve">D. Morton and C. Duriyanga. The Traditional Music of Thailand, volume 8. Univ of California Press, 1976</t>
   </si>
   <si>
+    <t xml:space="preserve">Monochord &amp; Stroboconn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mentions methods of playing simultaneous octaves: “kro” and “kep”.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Joerg Haeberli. Twelve nasca panpipes: A study. Ethnomusicology, 23(1):57–74, 1979. doi: 10.2307/851338</t>
   </si>
   <si>
+    <t xml:space="preserve">The interval between the first note and its overblown harmonic is not included for consistency (since only the overblown harmonic for one note is reported)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is not know whether overblown harmonics were used by the original players.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gerhard Kubik. Likembe tunings of kufuna kandonga (angola). Afr. Music, 6(1):70–88, 1980</t>
   </si>
   <si>
+    <t xml:space="preserve">Mentions singing in parallel octaves. Likembe is tuned consistently to within 9 Hz of an octave.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 Tunings taken from the same instrument, tuned by the same player on different days. “Kufuna has never shown any sign that he conceived of more than precisely one tuning pattern for his likembe. He always tuned his instrument to the same hexa- tonic scale, though with certain objectively measurable fluctuations in the intervals. These fluctuations, however, occurred within a clearly delimited margin of tolerance that was intra-culturally acceptable to him.”</t>
+  </si>
+  <si>
     <t xml:space="preserve">W. Van Zanten. The equidistant heptatonic scale of the asena in malawi. Afr. Music, 6(1):107–125, 1980. doi: 10.21504/amj. V6i1.1099</t>
   </si>
   <si>
+    <t xml:space="preserve">Tuning forks; measurement error noted as 9 cents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part of the tuning procedure is to “check the octaves”.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hugo Zemp. Melanesian solo polyphonic panpipe music. Ethnomusicology, 25(3):383–418, 1981. doi: 10.2307/851551</t>
   </si>
   <si>
+    <t xml:space="preserve">Evidence that parallel octaves are played, and they have a name for the octave: “the octaves were blown in parallel by two instruments of different sizes”; “Sunai and To'ihi'ona from Hautahe were the only musicians who used this term for the relationship of an octave, the common designation being suri 'au or aano suri”</t>
+  </si>
+  <si>
     <t xml:space="preserve">B. A. Aning. Tuning the kora: A case study of the norms of a gambian musician. J. Afr. Stud., 9(3):164, 1982</t>
   </si>
   <si>
+    <t xml:space="preserve">Tuning forks; same range of tuning forks as [16]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The author writes about octaves in the tuning of the kora, and notes that many strings are an octave apart. However, deviations from the octave leave the author unsure about whether there is a systematically regular tuning pattern for the kora. However there are a remarkable number of strings tuned to within 20 cents of an octave. The author repeatedly neglects to take into account imprecision in both tuning fork measurements, and the human ear, as acceptable reasons for deviations from theoretical ideals.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ho Lu-Ting and Han Kuo-huang. On chinese scales and national modes. Asian Music, 14(1):132–154, 1982. doi: 10.2307/ 834047</t>
   </si>
   <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
     <t xml:space="preserve">Despite being written on Western staff notation, I have assumed that these scales follow the Shi-er-lu tuning system.</t>
   </si>
   <si>
+    <t xml:space="preserve">The author remarks little on the use of the octave, and seems to have a similar understanding to that of Western music theory. “The Chinese use wusheng, and qisheng liusheng, to denote and 7-tone 6-tone, 5-tone, yinjie scales These terms refer to the number of pitches respectively. within an octave.”</t>
+  </si>
+  <si>
     <t xml:space="preserve">G. Kubik. A structural examination of homophonic multi-part singing in east and central africa. Anuario Musical, 39:27, 1984</t>
   </si>
   <si>
+    <t xml:space="preserve">“the man’s and the woman’s vocal lines sometimes sound in octaves...”</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gerhard Kubik. African tone-systems: A reassessment. Yearb. Tradit. Music, 17:31–63, 1985. doi: 10.2307/768436</t>
   </si>
   <si>
+    <t xml:space="preserve">“The intervals struck simultaneously in the xylophone music of southern Cameroon are mainly thirds and octaves”</t>
+  </si>
+  <si>
     <t xml:space="preserve">Robert Gottlieb. Sudan ii: Music of the blue nile province; the ingessana and berta tribes, 1986</t>
   </si>
   <si>
+    <t xml:space="preserve">Not mentioned. Intervals are measured to the nearest 1 cent.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“This may be an intentional stretching of the octave since the same tuning is consistently used in performances”</t>
+  </si>
+  <si>
     <t xml:space="preserve">R. Yu-An, E. C. Carterette, and W. Yu-Kui. A comparison of the musical scales of the ancient chinese bronze bell ensemble and the modern bamboo flute. Percept. Psychophys., 41(6):547–562, 1987. doi: 10.3758/BF03210489</t>
   </si>
   <si>
+    <t xml:space="preserve">Briiel &amp; Kjaer Type 2300 High-Resolution Signal Analyzer; a group of listeners matched computer generated sine tones to the fundamental frequencies of the instruments.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No mention is made of how the instruments were played and whether octaves are prominent. The authors note that both flute and bells have a ‘true octave’.</t>
+  </si>
+  <si>
     <t xml:space="preserve">D. H. Keefe, E. M. Burns, and P. Nguyen. Vietnamese modal scales of the dan tranh. Music Percept., 8(4):449–468, 1991. doi: 10.2307/40285522</t>
   </si>
   <si>
+    <t xml:space="preserve">Peterson tuner; 1 cent accuracy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Traditional Vietnamese music, like many other music culture octave equivalence and uses a scale system with discrete pitch classes.”</t>
+  </si>
+  <si>
     <t xml:space="preserve">A. Tracey. Kambazithe makolekole and his valimba group: A glimpse of the technique of the sena xylophone. Afr. Music, 7 (1):82–104, 1991. doi: 10.21504/amj.v7i1.1932</t>
   </si>
   <si>
+    <t xml:space="preserve">It is noted of the player/tuner that “he checks octaves” while tuning.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Edward C. Carterette, Roger A. Kendall, and Sue Carole De Vale. Comparative acoustical and psychoacoustical analyses of gamelan instrument tones. Journal of the Acoustical Society of Japan (E), 14(6):383–396, 1993. doi: 10.1250/ast.14.383</t>
   </si>
   <si>
+    <t xml:space="preserve">Hewlett-Packard 5512A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stretched octaves have been well-documented in Gamelan music, and the octave is repeatedly referred to here.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Albrecht Schneider. Sound, pitch, and scale: From ”tone measurements” to sonological analysis in ethnomusicology. Ethno- musicology, 45(3):489–519, 2001. doi: 10.2307/852868</t>
   </si>
   <si>
+    <t xml:space="preserve">Computational</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stretched octaves have been well-documented in Gamelan music.</t>
+  </si>
+  <si>
     <t xml:space="preserve">K. Attakitmongcol, R. Chinvejkitvanich, and S. Sujitjorn. Characterization of traditional thai musical scale. In Proceedings of the 5th WSEAS International Conference on Acoustics and Music: Theory &amp; Applications (AMTA04), 2004</t>
   </si>
   <si>
+    <t xml:space="preserve">Refers to Thai octave; notes that the octave is used in theory.</t>
+  </si>
+  <si>
     <t xml:space="preserve">J. Zhang, X. Xiao, and Y. K. Lee. The early development of music. analysis of the jiahu bone flutes. Antiquity, 78(302): 769778, 2004. doi: 10.1017/S0003598X00113432</t>
   </si>
   <si>
     <t xml:space="preserve">Despite recording cents to an accuracy of 1 cent, many intervals fall on exact 12-TET intervals. Given the leeway in tuning for flutes this looks like a potential case of bias on part of the researchers. Nonetheless, I reserve judgment and include the scales.</t>
   </si>
   <si>
+    <t xml:space="preserve">Not possible to establish for these prehistoric flutes.</t>
+  </si>
+  <si>
     <t xml:space="preserve">W. A. Sethares. Tuning, Timbre, Spectrum, Scale. Springer Science &amp; Business Media, 2005</t>
   </si>
   <si>
     <t xml:space="preserve">L. E. McNeil and S. Mitran. Vibrational frequencies and tuning of the african mbira. J. Acoust. Soc. Am., 123(2):1169–1178, 2008. doi: 10.1121/1.2828063</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Korg AT-12 Auto Chromatic tuner</t>
   </si>
   <si>
     <t xml:space="preserve">Multiple octaves were recorded as separate scales for each xylophone for two reasons.
@@ -3954,7 +4101,13 @@
 Second, there is substantial variation between octaves to consider them as distinct versions of the same scale.</t>
   </si>
   <si>
+    <t xml:space="preserve">Pitches tend to have the same name across multiple octaves (with the exception of the ‘baana’ pitch)</t>
+  </si>
+  <si>
     <t xml:space="preserve">M. Kuss. Music in Latin America and the Caribbean: An Encyclopedic History: Volume 1: Performing Beliefs: Indigenous Peoples of South America, Central America, and Mexico. University of Texas Press, 2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">… lost access… must buy the book to obtain info</t>
   </si>
   <si>
     <r>
@@ -3987,22 +4140,40 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">“However, many tuners do not intend to tune the octave to a ratio of 1:2, but aim for a marginally larger interval.” Marginally here meaning about 10 cents.</t>
+  </si>
+  <si>
     <t xml:space="preserve">N. Wisuttipat. Relative nature of thai traditional music through its tuning system. International Journal of Creative and Arts Studies, 2(1):86–97, 2015. doi: 10.24821/ijcas.v2i1.1441</t>
   </si>
   <si>
+    <t xml:space="preserve">Electronic tuner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See above for references on Thai music.</t>
+  </si>
+  <si>
     <t xml:space="preserve">A. Morkonr, S. Punkubutra, et al. The collecting process of xylophone’s sound d (ranād xek) from art to numerical data. In 2018 International Conference on Engineering, Applied Sciences, and Technology (ICEAST), pages 1–4, 2018. doi: 10.1109/ ICEAST.2018.8434434</t>
   </si>
   <si>
     <t xml:space="preserve">R. Bader. Temperament in tuning systems of southeast asia and ancient india. In Computational Phonogram Archiving, pages 75–107. Springer, 2019. doi: 10.1007/978-3-030-02695-0 3</t>
   </si>
   <si>
+    <t xml:space="preserve">The author measured the tuning of Cambodian instruments bought in Russia… no mention is made of the original performers.</t>
+  </si>
+  <si>
     <t xml:space="preserve">C. M. L. Kimberlin. Masinqo and the Nature of Qanat. PhD thesis, 1976</t>
   </si>
   <si>
     <t xml:space="preserve">Inferred from recordings</t>
   </si>
   <si>
+    <t xml:space="preserve">“Qanat is an interval set which consists of five basic pitches plus the octave and provides the tonal basis for any musical composition.”</t>
+  </si>
+  <si>
     <t xml:space="preserve">Unjung Nam. Pitch distributions in korean court music: Evidence consistent with tonal hierarchies. Music Percept., 16(2): 243–247, 1998. doi: 10.2307/40285789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author barely discusses the octave.</t>
   </si>
   <si>
     <t xml:space="preserve">S. Weisser and F. Falceto. Investigating qanat in amhara secular music: An acoustic and historical study. Annales d’thiopie, 28(1):299–322, 2013. doi: 10.3406/ethio.2013.1539</t>
@@ -4010,6 +4181,9 @@
   <si>
     <t xml:space="preserve">Despite noting in the text that the octave, the final interval leading to the octave is not reported. In this case I assume that the octave is perfect, and insert the missing interval.
 Inferred from recordings </t>
+  </si>
+  <si>
+    <t xml:space="preserve">See reference [38] for discussion of qanat</t>
   </si>
   <si>
     <t xml:space="preserve">Reasons for not using sources</t>
@@ -4083,12 +4257,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -4139,7 +4319,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4184,8 +4364,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -4197,6 +4393,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFF200"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -4207,7 +4463,7 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -4312,7 +4568,7 @@
   </sheetPr>
   <dimension ref="A1:I467"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A351" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A351" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H355" activeCellId="0" sqref="H355"/>
     </sheetView>
   </sheetViews>
@@ -17887,7 +18143,7 @@
   </sheetPr>
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I42" activeCellId="0" sqref="I42"/>
     </sheetView>
   </sheetViews>
@@ -19542,8 +19798,8 @@
   </sheetPr>
   <dimension ref="A1:GZ31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="FY1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="GK9" activeCellId="0" sqref="GK9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="EK1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="FA7" activeCellId="0" sqref="FA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29777,7 +30033,7 @@
   </sheetPr>
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M53" activeCellId="0" sqref="M53"/>
     </sheetView>
   </sheetViews>
@@ -32094,7 +32350,7 @@
   </sheetPr>
   <dimension ref="A1:BB21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K35" activeCellId="0" sqref="K35"/>
     </sheetView>
   </sheetViews>
@@ -34591,382 +34847,731 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="283.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="221.89"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="54.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="12" width="71.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="12" width="86.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="12" width="25.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="12" width="108"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="12" width="88.1"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="12" t="s">
         <v>1270</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="12" t="s">
         <v>1271</v>
       </c>
+      <c r="D1" s="12" t="s">
+        <v>1272</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>1273</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>1274</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>1275</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>1272</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+      <c r="B2" s="12" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>1273</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>1274</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
+      <c r="B3" s="12" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>1279</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>1275</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>1276</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
+      <c r="B4" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>1281</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="12" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>1283</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>1283</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>1288</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>1289</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>1290</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>1292</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>1294</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>1289</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="14" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>1296</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>1297</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>1277</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>1278</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>1279</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>1167</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>1170</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>1280</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="n">
+      <c r="F9" s="12" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="13" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>1281</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="n">
+      <c r="B10" s="12" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>1294</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>1289</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="13" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>1282</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="n">
+      <c r="B11" s="12" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>1294</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>1289</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="13" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="5" t="s">
         <v>1168</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="n">
+      <c r="C12" s="5" t="s">
+        <v>1302</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="14" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="15" t="s">
+        <v>1303</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="13" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>1305</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="13" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>1307</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>1283</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" s="0" t="s">
+      <c r="D15" s="12" t="s">
+        <v>1308</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>1289</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="13" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>1310</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>1283</v>
+      </c>
+      <c r="E16" s="12" t="s">
         <v>1284</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>1285</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>1286</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="n">
+      <c r="F16" s="12" t="s">
+        <v>1311</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="13" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="0" t="s">
-        <v>1287</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="n">
+      <c r="B17" s="12" t="s">
+        <v>1313</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>1314</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="13" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="12" t="s">
+        <v>1316</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>1283</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="13" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>1318</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>1319</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="13" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="13" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>1283</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="13" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>1327</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>1319</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="13" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>1329</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>1330</v>
+      </c>
+      <c r="D23" s="12" t="s">
         <v>1288</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" s="0" t="s">
+      <c r="E23" s="12" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="13" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>1332</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>1333</v>
+      </c>
+      <c r="E24" s="12" t="s">
         <v>1289</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11" t="n">
-        <v>19</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>1290</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>1291</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11" t="n">
-        <v>20</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>1292</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11" t="n">
-        <v>21</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>1293</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11" t="n">
-        <v>22</v>
-      </c>
-      <c r="B23" s="0" t="s">
+      <c r="F24" s="12" t="s">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="13" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>1335</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>1288</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="13" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>1338</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>1319</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="13" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>1340</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>1341</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="13" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>1343</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>1344</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>1289</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="13" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>1346</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>1344</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="13" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>1348</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>1283</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>1349</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>1289</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="13" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>1351</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>1344</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>1289</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="13" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>1352</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>1344</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="13" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>1353</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>1354</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="13" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>1357</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>1289</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="13" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>1358</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>1344</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="13" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>1361</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="13" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>1344</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="13" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>1364</v>
+      </c>
+      <c r="C38" s="12" t="s">
         <v>1294</v>
       </c>
-      <c r="C23" s="0" t="s">
-        <v>1279</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="11" t="n">
-        <v>23</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="11" t="n">
-        <v>24</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>1296</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>1279</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="11" t="n">
-        <v>25</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>1297</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="11" t="n">
-        <v>26</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>1298</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="11" t="n">
-        <v>27</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>1299</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="11" t="n">
-        <v>28</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="11" t="n">
-        <v>29</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>1301</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>1302</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="11" t="n">
-        <v>30</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>1303</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="11" t="n">
-        <v>31</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>1304</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="36.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="11" t="n">
-        <v>32</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>1166</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>1305</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11" t="n">
-        <v>33</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>1306</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="11" t="n">
-        <v>34</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>1307</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="11" t="n">
-        <v>35</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>1308</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="11" t="n">
-        <v>36</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="11" t="n">
-        <v>37</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>1310</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="11" t="n">
+      <c r="E38" s="12" t="s">
+        <v>1289</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="13" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="0" t="s">
-        <v>1311</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>1312</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="11" t="n">
+      <c r="B39" s="12" t="s">
+        <v>1366</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>1367</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="13" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="0" t="s">
-        <v>1313</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>1312</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="11" t="n">
+      <c r="B40" s="12" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>1367</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>1289</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="13" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="0" t="s">
-        <v>1314</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>1315</v>
+      <c r="B41" s="12" t="s">
+        <v>1371</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>1372</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>1373</v>
       </c>
     </row>
   </sheetData>
@@ -34987,7 +35592,7 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -35000,7 +35605,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
-        <v>1316</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35008,7 +35613,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1317</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35016,7 +35621,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>1318</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35024,7 +35629,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>1319</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35032,7 +35637,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>1320</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35040,7 +35645,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>1321</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35048,7 +35653,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>1322</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35056,7 +35661,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>1323</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35064,7 +35669,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>1324</v>
+        <v>1382</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated scales database text; added analyses and figures
</commit_message>
<xml_diff>
--- a/Scales_database/scales_database.xlsx
+++ b/Scales_database/scales_database.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6001" uniqueCount="1383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6022" uniqueCount="1387">
   <si>
     <t xml:space="preserve">Sheet</t>
   </si>
@@ -3848,19 +3848,25 @@
     <t xml:space="preserve">Notes on the inclusion of scales in the database</t>
   </si>
   <si>
-    <t xml:space="preserve">Supports octave equivalence</t>
+    <t xml:space="preserve">Players exhibit octave?</t>
   </si>
   <si>
     <t xml:space="preserve">Notes on octave equivalence</t>
   </si>
   <si>
+    <t xml:space="preserve">Sources indicate that octave is generally used in culture?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Other Notes</t>
   </si>
   <si>
     <t xml:space="preserve">M. J. Hewitt. Musical Scales of the World. Note Tree, 2013</t>
   </si>
   <si>
-    <t xml:space="preserve">?</t>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Too many cultures, too little information</t>
   </si>
   <si>
     <t xml:space="preserve">H. Rechberger. Scales and Modes Around the World: The Complete Guide to the Scales and Modes of the World. Fennica Gehrman Ltd., 2018</t>
@@ -3901,31 +3907,31 @@
     <t xml:space="preserve">Despite noting in the text that the octave, the final interval leading to the octave is not reported. In this case I assume that the octave is perfect, and insert the missing interval.</t>
   </si>
   <si>
+    <t xml:space="preserve">“Contrary movement from unison into octave and the reverse is a frequent practice in Azande harp music”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Each player seems to tune his instrument to fit best the range of his voice and that of the choir”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monochord</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“If men and women sing together the result is generally in parallel octaves”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not mentioned clearly</t>
+  </si>
+  <si>
     <t xml:space="preserve">No</t>
   </si>
   <si>
-    <t xml:space="preserve">“Contrary movement from unison into octave and the reverse is a frequent practice in Azande harp music”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“Each player seems to tune his instrument to fit best the range of his voice and that of the choir”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monochord</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“If men and women sing together the result is generally in parallel octaves”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not mentioned clearly</t>
-  </si>
-  <si>
     <t xml:space="preserve">“Seldom does the interval go beyond one full tone and rarely does the compass of a song contain more than one octave.”</t>
   </si>
   <si>
     <t xml:space="preserve">Gilbert Rouget and J. Schwarz. Sur les xylophones quiheptaphoniques des malink. Rev. Musicol., 55(1):47–77, 1969. doi: 10.2307/927751</t>
   </si>
   <si>
-    <t xml:space="preserve">French.. ask Francois</t>
+    <t xml:space="preserve">The author measured the tuning of instruments and remarks that the tuning conforms to a heptatonic scale such that notes are an octave apart; no mention is made of the original performers.</t>
   </si>
   <si>
     <t xml:space="preserve">A. Tracey. The matepe mbira music of rhodesia. Afr. Music, 4(4):37–61, 1970. doi: 10.21504/amj.v4i4.1681</t>
@@ -3946,6 +3952,15 @@
     <t xml:space="preserve">W. Surjodiningrat, A. Susanto, and P. J. Sudarjana. Tone Measurements of Outstanding Javanese Gamelans in Jogjakarta and Surakarta. Gadjah Mada University Press, 1972</t>
   </si>
   <si>
+    <t xml:space="preserve">Electronic / numerical analysis; “frequency differences of about 0.1 percent were easily detected”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authors mention that they expected notes to be separated by octaves, and note that this is often the case. However, what is described as ‘octave deviations’ are found to be as great as 63 cents.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes; REF</t>
+  </si>
+  <si>
     <t xml:space="preserve">D. Morton and C. Duriyanga. The Traditional Music of Thailand, volume 8. Univ of California Press, 1976</t>
   </si>
   <si>
@@ -3994,13 +4009,11 @@
     <t xml:space="preserve">Tuning forks; same range of tuning forks as [16]</t>
   </si>
   <si>
-    <t xml:space="preserve">The author writes about octaves in the tuning of the kora, and notes that many strings are an octave apart. However, deviations from the octave leave the author unsure about whether there is a systematically regular tuning pattern for the kora. However there are a remarkable number of strings tuned to within 20 cents of an octave. The author repeatedly neglects to take into account imprecision in both tuning fork measurements, and the human ear, as acceptable reasons for deviations from theoretical ideals.</t>
+    <t xml:space="preserve">The author writes about octaves in the tuning of the kora, and notes that many strings are an octave apart. However, deviations from the octave leave the author unsure about whether there is a systematically regular tuning pattern for the kora. However there are a remarkable number of strings tuned to within 20 cents of an octave. The author repeatedly neglects to take into account imprecision in both tuning fork measurements, and the human ear, as acceptable reasons for deviations from theoretical ideals.
+Incidentally, it is noted that the tuner pays particular attention to the intonation of two sets of strings, each a fifth apart.</t>
   </si>
   <si>
     <t xml:space="preserve">Ho Lu-Ting and Han Kuo-huang. On chinese scales and national modes. Asian Music, 14(1):132–154, 1982. doi: 10.2307/ 834047</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N/A</t>
   </si>
   <si>
     <t xml:space="preserve">Despite being written on Western staff notation, I have assumed that these scales follow the Shi-er-lu tuning system.</t>
@@ -4101,7 +4114,7 @@
 Second, there is substantial variation between octaves to consider them as distinct versions of the same scale.</t>
   </si>
   <si>
-    <t xml:space="preserve">Pitches tend to have the same name across multiple octaves (with the exception of the ‘baana’ pitch)</t>
+    <t xml:space="preserve">Pitches tend to have the same name across multiple octaves (with the exception of the ‘baana’ pitch); this seems like evidence of equivalence on the part of the performers.</t>
   </si>
   <si>
     <t xml:space="preserve">M. Kuss. Music in Latin America and the Caribbean: An Encyclopedic History: Volume 1: Performing Beliefs: Indigenous Peoples of South America, Central America, and Mexico. University of Texas Press, 2010</t>
@@ -4257,18 +4270,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFF200"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -4319,7 +4326,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4376,14 +4383,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -4393,66 +4392,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFF200"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -34847,10 +34786,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -34861,31 +34800,34 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="12" width="86.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="12" width="25.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="12" width="108"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="12" width="88.1"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="12" width="88.1"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="4" t="s">
         <v>1270</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="4" t="s">
         <v>1271</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="4" t="s">
         <v>1272</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="4" t="s">
         <v>1273</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="4" t="s">
         <v>1274</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="4" t="s">
         <v>1275</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>1276</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34893,38 +34835,56 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>1276</v>
-      </c>
-      <c r="E2" s="12" t="s">
         <v>1277</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="5" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>1279</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>1281</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>1278</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="F3" s="12" t="s">
         <v>1279</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>1277</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G3" s="5" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>1280</v>
+        <v>1282</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>1281</v>
+        <v>1283</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>1277</v>
+        <v>1278</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>1279</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>1278</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34932,19 +34892,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>1282</v>
+        <v>1284</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>1283</v>
+        <v>1285</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>1285</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>1286</v>
+        <v>1287</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>1288</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34952,22 +34912,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>1287</v>
+        <v>1289</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>1283</v>
+        <v>1285</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>1288</v>
+        <v>1290</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>1289</v>
+        <v>1286</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>1290</v>
-      </c>
-      <c r="G6" s="12" t="s">
         <v>1291</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>1292</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34978,13 +34938,13 @@
         <v>1167</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34995,67 +34955,67 @@
         <v>1170</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>1289</v>
+        <v>1296</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>1295</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="n">
+      <c r="A9" s="13" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="5" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>1285</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>1296</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>1297</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>1277</v>
-      </c>
       <c r="F9" s="12" t="s">
-        <v>1297</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>1298</v>
+        <v>1300</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>1289</v>
+        <v>1286</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>1299</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>1300</v>
+        <v>1302</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>1289</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1296</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="n">
         <v>11</v>
       </c>
@@ -35063,21 +35023,30 @@
         <v>1168</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>1302</v>
+        <v>1304</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>1289</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="n">
+      <c r="A13" s="13" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>1303</v>
+      <c r="B13" s="5" t="s">
+        <v>1305</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>1306</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>1277</v>
+        <v>1296</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>1307</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>1308</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35085,36 +35054,36 @@
         <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>1304</v>
+        <v>1309</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>1305</v>
+        <v>1310</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>1306</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>1307</v>
+        <v>1312</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>1283</v>
+        <v>1285</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>1308</v>
+        <v>1313</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>1289</v>
+        <v>1296</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>1309</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35122,19 +35091,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>1310</v>
+        <v>1315</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>1283</v>
+        <v>1285</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>1311</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>1312</v>
+        <v>1316</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>1317</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35142,16 +35111,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>1313</v>
+        <v>1318</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>1314</v>
+        <v>1319</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>1315</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35159,33 +35128,33 @@
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>1316</v>
+        <v>1321</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>1283</v>
+        <v>1285</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>1317</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="n">
         <v>18</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>1318</v>
+        <v>1323</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>1319</v>
+        <v>1324</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>1284</v>
+        <v>1296</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>1320</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35193,53 +35162,56 @@
         <v>19</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>1321</v>
+        <v>1326</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>1322</v>
+        <v>1278</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>1323</v>
+        <v>1327</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>1284</v>
+        <v>1296</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>1324</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1328</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="n">
         <v>20</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>1325</v>
+        <v>1329</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>1283</v>
+        <v>1285</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>1326</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="13" t="n">
         <v>21</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>1327</v>
+        <v>1331</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>1319</v>
+        <v>1324</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>1328</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35247,56 +35219,59 @@
         <v>22</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>1329</v>
+        <v>1333</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>1330</v>
+        <v>1334</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>1288</v>
+        <v>1290</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>1331</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="13" t="n">
         <v>23</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>1332</v>
+        <v>1336</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>1333</v>
+        <v>1337</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>1289</v>
+        <v>1296</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>1334</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="13" t="n">
         <v>24</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>1335</v>
+        <v>1339</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>1336</v>
+        <v>1340</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>1288</v>
+        <v>1290</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>1337</v>
+        <v>1341</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>1308</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35304,33 +35279,36 @@
         <v>25</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>1338</v>
+        <v>1342</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>1319</v>
+        <v>1324</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>1339</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="13" t="n">
         <v>26</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>1340</v>
+        <v>1344</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>1341</v>
+        <v>1345</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>1284</v>
+        <v>1296</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>1342</v>
+        <v>1346</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>1308</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35338,53 +35316,59 @@
         <v>27</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>1343</v>
+        <v>1347</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>1344</v>
+        <v>1348</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>1289</v>
+        <v>1296</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>1345</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1349</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="13" t="n">
         <v>28</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>1346</v>
+        <v>1350</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>1344</v>
+        <v>1348</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>1284</v>
+        <v>1296</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>1347</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1351</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="13" t="n">
         <v>29</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>1348</v>
+        <v>1352</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>1283</v>
+        <v>1285</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>1349</v>
+        <v>1353</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>1289</v>
+        <v>1296</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>1350</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35392,30 +35376,33 @@
         <v>30</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>1351</v>
+        <v>1355</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>1344</v>
+        <v>1348</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>1289</v>
+        <v>1296</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>1345</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1349</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="13" t="n">
         <v>31</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>1352</v>
+        <v>1356</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>1344</v>
+        <v>1348</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>1289</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35426,67 +35413,70 @@
         <v>1166</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>1353</v>
+        <v>1357</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>1354</v>
+        <v>1358</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>1355</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="13" t="n">
         <v>33</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>1356</v>
+        <v>1360</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>1357</v>
+        <v>1361</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>1289</v>
+        <v>1296</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>1357</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="13" t="n">
         <v>34</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>1358</v>
+        <v>1362</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>1344</v>
+        <v>1348</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>1284</v>
+        <v>1296</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>1359</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="13" t="n">
         <v>35</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>1360</v>
+        <v>1364</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>1361</v>
+        <v>1365</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>1284</v>
+        <v>1296</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>1362</v>
+        <v>1366</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>1308</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35494,50 +35484,56 @@
         <v>36</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>1363</v>
+        <v>1367</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>1344</v>
+        <v>1348</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>1284</v>
+        <v>1296</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>1362</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1366</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="13" t="n">
         <v>37</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>1364</v>
+        <v>1368</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>1289</v>
+        <v>1296</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>1365</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="13" t="n">
         <v>38</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>1366</v>
+        <v>1370</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>1367</v>
+        <v>1371</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>1368</v>
+        <v>1372</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>1308</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35545,33 +35541,39 @@
         <v>39</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>1369</v>
+        <v>1373</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>1367</v>
+        <v>1371</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>1289</v>
+        <v>1296</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1374</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="13" t="n">
         <v>40</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>1371</v>
+        <v>1375</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>1372</v>
+        <v>1376</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>1373</v>
+        <v>1377</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>1308</v>
       </c>
     </row>
   </sheetData>
@@ -35605,7 +35607,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
-        <v>1374</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35613,7 +35615,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1375</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35621,7 +35623,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>1376</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35629,7 +35631,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>1377</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35637,7 +35639,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>1378</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35645,7 +35647,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>1379</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35653,7 +35655,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>1380</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35661,7 +35663,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>1381</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35669,7 +35671,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>1382</v>
+        <v>1386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated use of octave textual analysis
</commit_message>
<xml_diff>
--- a/Scales_database/scales_database.xlsx
+++ b/Scales_database/scales_database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12518" uniqueCount="2026">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12683" uniqueCount="2032">
   <si>
     <t xml:space="preserve">Sheet</t>
   </si>
@@ -5694,6 +5694,15 @@
   </si>
   <si>
     <t xml:space="preserve">Sources indicate that octave is generally used in culture?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuning octaves?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note name octaves?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parallel octaves?</t>
   </si>
   <si>
     <t xml:space="preserve">Other Notes</t>
@@ -5785,6 +5794,9 @@
     <t xml:space="preserve">5 cents resolution given, but no measurement device specified</t>
   </si>
   <si>
+    <t xml:space="preserve">No mention of the octave</t>
+  </si>
+  <si>
     <t xml:space="preserve">W. Surjodiningrat, A. Susanto, and P. J. Sudarjana. Tone Measurements of Outstanding Javanese Gamelans in Jogjakarta and Surakarta. Gadjah Mada University Press, 1972</t>
   </si>
   <si>
@@ -5821,7 +5833,7 @@
     <t xml:space="preserve">Mentions singing in parallel octaves. Likembe is tuned consistently to within 9 Hz of an octave.</t>
   </si>
   <si>
-    <t xml:space="preserve">5 Tunings taken from the same instrument, tuned by the same player on different days. “Kufuna has never shown any sign that he conceived of more than precisely one tuning pattern for his likembe. He always tuned his instrument to the same hexa- tonic scale, though with certain objectively measurable fluctuations in the intervals. These fluctuations, however, occurred within a clearly delimited margin of tolerance that was intra-culturally acceptable to him.”</t>
+    <t xml:space="preserve">5 Tunings taken from the same instrument, tuned by the same player on different days. “Kufuna has never shown any sign that he conceived of more than precisely one tuning pattern for his likembe. He always tuned his instrument to the same hexa- tonic scale, though with certain objectively measurable fluctuations in the intervals. These fluctuations, however, occurred within a clearly delimited margin of tolerance that was intra-culturally acceptable to him.” It’s also curious to hear that the author does not seem to mind the differences in tuning, despite being able to perceive them.</t>
   </si>
   <si>
     <t xml:space="preserve">W. Van Zanten. The equidistant heptatonic scale of the asena in malawi. Afr. Music, 6(1):107–125, 1980. doi: 10.21504/amj. V6i1.1099</t>
@@ -5868,6 +5880,9 @@
   </si>
   <si>
     <t xml:space="preserve">“The intervals struck simultaneously in the xylophone music of southern Cameroon are mainly thirds and octaves”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Describes notes in a scale using numbers; then upper and lower octaves are called “husbands” and “wives”</t>
   </si>
   <si>
     <t xml:space="preserve">Robert Gottlieb. Sudan ii: Music of the blue nile province; the ingessana and berta tribes, 1986</t>
@@ -6150,10 +6165,13 @@
     <t xml:space="preserve">Author discusses playing of the second harmonics, corresponding to an octave above the fundamental.</t>
   </si>
   <si>
+    <t xml:space="preserve">The author speculates, but no mention is made of how the instruments were played.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See Guillermo Abadia Morales</t>
+  </si>
+  <si>
     <t xml:space="preserve">No mention is made of how the instruments were played.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">See Guillermo Abadia Morales</t>
   </si>
   <si>
     <t xml:space="preserve">This source only provided absolute frequencies for notes in some recorded songs, along with transcriptions. I myself converted these into exact scales; methodology and code will be published somewhere.</t>
@@ -6510,10 +6528,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
-        <v>2016</v>
+        <v>2022</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2017</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6521,7 +6539,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>2018</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6529,7 +6547,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>2019</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6537,7 +6555,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>2020</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6545,7 +6563,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>2021</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6553,7 +6571,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>2022</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6561,7 +6579,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>2023</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6569,7 +6587,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>2024</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6577,7 +6595,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>2025</v>
+        <v>2031</v>
       </c>
     </row>
   </sheetData>
@@ -6771,8 +6789,8 @@
   </sheetPr>
   <dimension ref="A1:P467"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -33348,8 +33366,8 @@
   </sheetPr>
   <dimension ref="A1:AK240"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A165" activeCellId="0" sqref="A165"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A163" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A180" activeCellId="0" sqref="A180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -51909,10 +51927,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -51923,8 +51943,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="86.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="25.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="108"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="5" width="88.1"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="5" width="88.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="5" width="22.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="88.1"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51952,21 +51976,39 @@
       <c r="H1" s="6" t="s">
         <v>1888</v>
       </c>
+      <c r="I1" s="6" t="s">
+        <v>1889</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>1890</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>1891</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1889</v>
+        <v>1892</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>62</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>1890</v>
+        <v>1893</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>62</v>
       </c>
     </row>
@@ -51975,18 +52017,27 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1891</v>
+        <v>1894</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>1892</v>
+        <v>1895</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>62</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>1890</v>
+        <v>1893</v>
       </c>
       <c r="G3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>62</v>
       </c>
     </row>
@@ -51995,39 +52046,57 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>1896</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>1897</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>1893</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>1894</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>1890</v>
-      </c>
       <c r="G4" s="5" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1895</v>
+        <v>1898</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>1896</v>
+        <v>1899</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>1897</v>
+        <v>1900</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>1898</v>
+        <v>1901</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>1899</v>
+        <v>1900</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>1902</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52035,22 +52104,31 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>1903</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>1899</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>1904</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>1900</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>1896</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>1901</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>1897</v>
-      </c>
       <c r="F6" s="5" t="s">
-        <v>1902</v>
+        <v>1905</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>1903</v>
+        <v>62</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>1900</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>1906</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52061,13 +52139,22 @@
         <v>1481</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>1904</v>
+        <v>1907</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>1897</v>
+        <v>1900</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>1905</v>
+        <v>1908</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>1900</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52078,30 +52165,48 @@
         <v>1520</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>1906</v>
+        <v>1909</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>1908</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1911</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>1910</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>1910</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>1909</v>
+        <v>1912</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>1896</v>
+        <v>1899</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>1910</v>
+        <v>1913</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52109,16 +52214,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>1911</v>
+        <v>1914</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>1906</v>
+        <v>1909</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>1897</v>
+        <v>1900</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>1912</v>
+        <v>1915</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>1900</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52126,19 +52240,28 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>1913</v>
+        <v>1916</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>1906</v>
+        <v>1909</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>1914</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1910</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="n">
         <v>11</v>
       </c>
@@ -52146,10 +52269,22 @@
         <v>1505</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>1915</v>
+        <v>1918</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>1919</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52157,19 +52292,31 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>1916</v>
+        <v>1920</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>1917</v>
+        <v>1921</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>1918</v>
+        <v>1922</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>1919</v>
+        <v>1923</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52177,73 +52324,109 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1920</v>
+        <v>1924</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>1921</v>
+        <v>1925</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>1897</v>
+        <v>1900</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>1922</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1926</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>1923</v>
+        <v>1927</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>1896</v>
+        <v>1899</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>1924</v>
+        <v>1928</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>1925</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1929</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>1926</v>
+        <v>1930</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>1896</v>
+        <v>1899</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>1897</v>
+        <v>1900</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>1927</v>
+        <v>1931</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>1928</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1910</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>1900</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>1932</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>1929</v>
+        <v>1933</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>1930</v>
+        <v>1934</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>1897</v>
+        <v>1900</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>1931</v>
+        <v>1935</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>1900</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52251,33 +52434,51 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>1932</v>
+        <v>1936</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>1896</v>
+        <v>1899</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>1897</v>
+        <v>1900</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>1933</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1937</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>1910</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>1900</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="n">
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1934</v>
+        <v>1938</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>1935</v>
+        <v>1939</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>1936</v>
+        <v>1940</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>1910</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52285,116 +52486,174 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>1937</v>
+        <v>1941</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>62</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>1938</v>
+        <v>1942</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>1939</v>
+        <v>1943</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>1919</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1923</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="n">
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>1940</v>
+        <v>1944</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>1896</v>
+        <v>1899</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>1897</v>
+        <v>1900</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>1941</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1945</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="13" t="n">
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1942</v>
+        <v>1946</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>1935</v>
+        <v>1939</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>1897</v>
+        <v>1900</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>1943</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1947</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>1900</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>1900</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>1900</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13" t="n">
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>1944</v>
+        <v>1949</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>1945</v>
+        <v>1950</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>1901</v>
+        <v>1904</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>1897</v>
+        <v>1900</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>1946</v>
-      </c>
+        <v>1951</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>1910</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="13" t="n">
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>1947</v>
+        <v>1952</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>1948</v>
+        <v>1953</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>1949</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1954</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="13" t="n">
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>1950</v>
+        <v>1955</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>1951</v>
+        <v>1956</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>1901</v>
+        <v>1904</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>1897</v>
+        <v>1900</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>1952</v>
+        <v>1957</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>1919</v>
+        <v>1923</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>1900</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52402,36 +52661,54 @@
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>1953</v>
+        <v>1958</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>1935</v>
+        <v>1939</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>1897</v>
+        <v>1900</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>1954</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1959</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>1900</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="13" t="n">
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>1955</v>
+        <v>1960</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>1956</v>
+        <v>1961</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>1957</v>
+        <v>1962</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>1919</v>
+        <v>1923</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52439,59 +52716,86 @@
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>1958</v>
+        <v>1963</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>1959</v>
+        <v>1964</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>1960</v>
+        <v>1965</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>1919</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1923</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="13" t="n">
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>1961</v>
+        <v>1966</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>1959</v>
+        <v>1964</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>1962</v>
+        <v>1967</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>1919</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1923</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>1900</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="13" t="n">
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>1963</v>
+        <v>1968</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>1896</v>
+        <v>1899</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>1964</v>
+        <v>1969</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>1965</v>
+        <v>1970</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52499,33 +52803,51 @@
         <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>1966</v>
+        <v>1971</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>1959</v>
+        <v>1964</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>1960</v>
+        <v>1965</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>1919</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1923</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="13" t="n">
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>1967</v>
+        <v>1972</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>1959</v>
+        <v>1964</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52536,36 +52858,54 @@
         <v>1470</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>1968</v>
+        <v>1973</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>1969</v>
+        <v>1974</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>1897</v>
+        <v>1900</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>1970</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1975</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>1900</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="13" t="n">
         <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>1971</v>
+        <v>1976</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>1972</v>
+        <v>1977</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>1973</v>
+        <v>1978</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>1897</v>
+        <v>1900</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>1974</v>
+        <v>1979</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>1900</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>1900</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52573,16 +52913,25 @@
         <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>1975</v>
+        <v>1980</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>1959</v>
+        <v>1964</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>1976</v>
+        <v>1981</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52590,16 +52939,25 @@
         <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>1977</v>
+        <v>1982</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>1978</v>
+        <v>1983</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>1897</v>
+        <v>1900</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>1979</v>
+        <v>1984</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52607,36 +52965,54 @@
         <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>1980</v>
+        <v>1985</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>1959</v>
+        <v>1964</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>1981</v>
+        <v>1986</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>1919</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1923</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="13" t="n">
         <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>1982</v>
+        <v>1987</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>1906</v>
+        <v>1909</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>1983</v>
+        <v>1988</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52644,19 +53020,28 @@
         <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>1984</v>
+        <v>1989</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>1985</v>
+        <v>1990</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>1897</v>
+        <v>1900</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>1986</v>
+        <v>1991</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>1919</v>
+        <v>1923</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52664,19 +53049,28 @@
         <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>1987</v>
+        <v>1992</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>1985</v>
+        <v>1990</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>1988</v>
+        <v>1993</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>1919</v>
+        <v>1923</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52684,22 +53078,31 @@
         <v>40</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>1989</v>
+        <v>1994</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>1990</v>
+        <v>1995</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>1897</v>
+        <v>1900</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>1991</v>
+        <v>1996</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>1919</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1923</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="8" t="n">
         <v>41</v>
       </c>
@@ -52707,19 +53110,28 @@
         <v>1544</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>1992</v>
+        <v>1997</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>1985</v>
+        <v>1990</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>1993</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1998</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="n">
         <v>42</v>
       </c>
@@ -52727,22 +53139,31 @@
         <v>1550</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>1994</v>
+        <v>1999</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>1985</v>
+        <v>1990</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>1993</v>
+        <v>1998</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>62</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K43" s="5" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="8" t="n">
         <v>43</v>
       </c>
@@ -52750,13 +53171,22 @@
         <v>1567</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>1896</v>
+        <v>1899</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>1996</v>
+        <v>2001</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52767,19 +53197,28 @@
         <v>1873</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>1906</v>
+        <v>1909</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>1997</v>
+        <v>2002</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>1897</v>
+        <v>1900</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>1998</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2003</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>1900</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>1900</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="8" t="n">
         <v>45</v>
       </c>
@@ -52787,19 +53226,28 @@
         <v>1572</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>1896</v>
+        <v>1899</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>1999</v>
+        <v>2004</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2005</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8" t="n">
         <v>46</v>
       </c>
@@ -52807,19 +53255,28 @@
         <v>1575</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>2001</v>
+        <v>2006</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>2002</v>
+        <v>2007</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>2003</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2008</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="8" t="n">
         <v>47</v>
       </c>
@@ -52827,19 +53284,28 @@
         <v>1600</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>2004</v>
+        <v>2009</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>2005</v>
+        <v>2010</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>2006</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>62</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J48" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K48" s="5" t="s">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="8" t="n">
         <v>48</v>
       </c>
@@ -52847,16 +53313,25 @@
         <v>1608</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>2004</v>
+        <v>2009</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>1897</v>
+        <v>1900</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>2007</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2012</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="8" t="n">
         <v>49</v>
       </c>
@@ -52864,13 +53339,22 @@
         <v>1612</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>2008</v>
+        <v>2013</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>1897</v>
+        <v>1900</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>2009</v>
+        <v>2014</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>1900</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>1900</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52881,13 +53365,22 @@
         <v>1615</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>2010</v>
+        <v>2015</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>1897</v>
+        <v>1900</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>2011</v>
+        <v>2016</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>1900</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52898,19 +53391,28 @@
         <v>1626</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>2010</v>
+        <v>2015</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>62</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="8" t="n">
         <v>52</v>
       </c>
@@ -52918,17 +53420,26 @@
         <v>1644</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>1959</v>
+        <v>1964</v>
       </c>
       <c r="D53" s="0"/>
       <c r="E53" s="5" t="s">
-        <v>1907</v>
+        <v>1910</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2019</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J53" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="8" t="n">
         <v>53</v>
       </c>
@@ -52936,16 +53447,25 @@
         <v>1651</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>1959</v>
+        <v>1964</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>2014</v>
+        <v>2020</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>1897</v>
+        <v>1900</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>2015</v>
+        <v>2021</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>